<commit_message>
Change to original muscles
</commit_message>
<xml_diff>
--- a/upper limb/inertial_parameters.xlsx
+++ b/upper limb/inertial_parameters.xlsx
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>thorax</t>
   </si>
   <si>
-    <t>mass</t>
-  </si>
-  <si>
-    <t>mass center</t>
-  </si>
-  <si>
-    <t>inertia</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -78,14 +69,27 @@
   </si>
   <si>
     <t>hand</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Mass (kg)</t>
+  </si>
+  <si>
+    <t>Mass Center (m)</t>
+  </si>
+  <si>
+    <t>Inertia (kg m^2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -116,10 +120,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,63 +408,69 @@
   <dimension ref="B1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B1" sqref="B1:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
       <c r="L2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>26.83</v>
       </c>
       <c r="D3" s="2">
@@ -492,9 +503,9 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
         <v>0.156</v>
       </c>
       <c r="D4" s="2">
@@ -527,9 +538,9 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
         <v>0.70396000000000003</v>
       </c>
       <c r="D5" s="2">
@@ -562,9 +573,9 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
         <v>1.9975700000000001</v>
       </c>
       <c r="D6" s="2">
@@ -597,9 +608,9 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
         <v>1.1052999999999999</v>
       </c>
       <c r="D7" s="2">
@@ -632,9 +643,9 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3">
         <v>0.23358999999999999</v>
       </c>
       <c r="D8" s="2">
@@ -667,9 +678,9 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
         <v>0.58189999999999997</v>
       </c>
       <c r="D9" s="2">

</xml_diff>